<commit_message>
chore: sem2 sem4 btech62 and sem4 bca62 update
</commit_message>
<xml_diff>
--- a/raw/time_tables/BCA(bca-62)/4/1.xlsx
+++ b/raw/time_tables/BCA(bca-62)/4/1.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\EVEN 2026\2 Year\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18161A18-EF03-4B22-8F23-5AA857A62644}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7545" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4 sem" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
   <si>
     <t>Bachelors of Computer Applications</t>
   </si>
@@ -228,9 +234,6 @@
     <t>LBCA1,BCA2,BCA 3 &amp;BCA 4(23B12CA211)-SUD/CR425</t>
   </si>
   <si>
-    <t>LBCA1,BCA2,BCA 3 &amp;BCA 4(23B12CA211)-DEP/CR501</t>
-  </si>
-  <si>
     <t>LBCA1,BCA2,BCA 3 &amp;BCA 4(23B12CA215)-KA/CR425</t>
   </si>
   <si>
@@ -258,9 +261,6 @@
     <t>TBCA3(23B61CA223)-TR502/SLK</t>
   </si>
   <si>
-    <t>TBCA2(23B61CA223)-TR424/AJP</t>
-  </si>
-  <si>
     <t>TBCA1(23B61CA223)-TR502/AJP</t>
   </si>
   <si>
@@ -273,18 +273,9 @@
     <t>Dr.Meenal Jani</t>
   </si>
   <si>
-    <t>PBCA4(23B65CA224) CC 421 SHV,NET</t>
-  </si>
-  <si>
-    <t>PBCA3(23B65CA225)/ CL13, CL14/ AJP,,PTK</t>
-  </si>
-  <si>
     <t>PBCA 4(23B65CA225)/ CL13,Cl14,/SKS,AJP</t>
   </si>
   <si>
-    <t>PBCA2(23B65CA224)CC417 KM,RTK</t>
-  </si>
-  <si>
     <t>PBCA1(23B65CA224  CL306,)SHR,RTK</t>
   </si>
   <si>
@@ -309,9 +300,6 @@
     <t>PBCA1(23B65CA225)/ CL01,SHP,AJP</t>
   </si>
   <si>
-    <t>PBCA 2(23B65CA225)CC417,/NET ,SKS,</t>
-  </si>
-  <si>
     <t>LBCA1,BCA2,BCA 3 &amp;BCA 4(23B12CA216)-MEE/CS6</t>
   </si>
   <si>
@@ -337,13 +325,28 @@
   </si>
   <si>
     <t>LBCA1,BCA2,BCA 3 &amp;BCA 4(23B12CA213)-DEP/CR501</t>
+  </si>
+  <si>
+    <t>PBCA 2(23B65CA225)CC417,/PTK ,SKS,</t>
+  </si>
+  <si>
+    <t>PBCA3(23B65CA225)/ CL13, CL14/ AJP,NET</t>
+  </si>
+  <si>
+    <t>PBCA4(23B65CA224) CC 421 RTK,NET</t>
+  </si>
+  <si>
+    <t>PBCA2(23B65CA224)CC417 SHR,RTK</t>
+  </si>
+  <si>
+    <t>TBCA2(23B61CA223)-TR502/AJP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="35">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,7 +576,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -610,6 +613,12 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -955,7 +964,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1134,9 +1143,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1152,81 +1158,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1235,9 +1166,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1248,6 +1176,102 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1508,18 +1532,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X993"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="124" zoomScaleNormal="106" zoomScaleSheetLayoutView="124" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="106" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
@@ -1533,18 +1557,18 @@
     <col min="10" max="24" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" customHeight="1">
-      <c r="A1" s="106" t="s">
+    <row r="1" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
       <c r="L1" s="18"/>
@@ -1561,18 +1585,18 @@
       <c r="W1" s="18"/>
       <c r="X1" s="18"/>
     </row>
-    <row r="2" spans="1:24" ht="21" customHeight="1">
-      <c r="A2" s="107" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
+    <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="121" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
       <c r="L2" s="18"/>
@@ -1589,7 +1613,7 @@
       <c r="W2" s="18"/>
       <c r="X2" s="18"/>
     </row>
-    <row r="3" spans="1:24" ht="19.5" customHeight="1" thickBot="1">
+    <row r="3" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19"/>
       <c r="B3" s="20" t="s">
         <v>1</v>
@@ -1616,59 +1640,59 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="68.25" customHeight="1" thickBot="1">
-      <c r="A4" s="108" t="s">
+    <row r="4" spans="1:24" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="76" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="69" t="s">
-        <v>103</v>
-      </c>
       <c r="E4" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="97" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="100" t="s">
-        <v>84</v>
-      </c>
-      <c r="I4" s="101"/>
+        <v>75</v>
+      </c>
+      <c r="H4" s="113" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="114"/>
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
     </row>
-    <row r="5" spans="1:24" ht="67.5" customHeight="1">
-      <c r="A5" s="108"/>
+    <row r="5" spans="1:24" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="122"/>
       <c r="B5" s="69" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="69" t="s">
-        <v>104</v>
-      </c>
       <c r="E5" s="69" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="77" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="F5" s="97"/>
+      <c r="G5" s="76" t="s">
+        <v>74</v>
       </c>
       <c r="H5" s="70"/>
       <c r="I5" s="70"/>
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="1:24" ht="10.5" customHeight="1">
+    <row r="6" spans="1:24" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
       <c r="B6" s="29"/>
       <c r="C6" s="30"/>
@@ -1681,51 +1705,51 @@
       <c r="J6" s="27"/>
       <c r="K6" s="27"/>
     </row>
-    <row r="7" spans="1:24" ht="58.5" customHeight="1">
-      <c r="A7" s="104" t="s">
+    <row r="7" spans="1:24" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="77" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>74</v>
+      <c r="B7" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="76" t="s">
+        <v>73</v>
       </c>
       <c r="D7" s="71"/>
       <c r="E7" s="71"/>
-      <c r="F7" s="86" t="s">
+      <c r="F7" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="77" t="s">
+      <c r="G7" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="77" t="s">
+      <c r="H7" s="76" t="s">
         <v>47</v>
       </c>
       <c r="I7" s="69" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
     </row>
-    <row r="8" spans="1:24" ht="60" customHeight="1">
-      <c r="A8" s="104"/>
-      <c r="B8" s="77" t="s">
+    <row r="8" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="118"/>
+      <c r="B8" s="76" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="71"/>
-      <c r="D8" s="100" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="101"/>
-      <c r="F8" s="86"/>
+      <c r="D8" s="113" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="114"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="72"/>
       <c r="H8" s="70"/>
       <c r="I8" s="70"/>
       <c r="J8" s="27"/>
       <c r="K8" s="27"/>
     </row>
-    <row r="9" spans="1:24" ht="12" customHeight="1">
+    <row r="9" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
@@ -1738,24 +1762,24 @@
       <c r="J9" s="27"/>
       <c r="K9" s="27"/>
     </row>
-    <row r="10" spans="1:24" ht="60.75" customHeight="1">
-      <c r="A10" s="105" t="s">
+    <row r="10" spans="1:24" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="100" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="101"/>
+      <c r="B10" s="116" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="117"/>
       <c r="D10" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="77" t="s">
+      <c r="E10" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="86" t="s">
+      <c r="F10" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="77" t="s">
+      <c r="G10" s="76" t="s">
         <v>47</v>
       </c>
       <c r="H10" s="73"/>
@@ -1765,22 +1789,22 @@
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
     </row>
-    <row r="11" spans="1:24" ht="56.25" customHeight="1">
-      <c r="A11" s="105"/>
-      <c r="B11" s="100" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="101"/>
+    <row r="11" spans="1:24" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="119"/>
+      <c r="B11" s="116" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="117"/>
       <c r="D11" s="71"/>
       <c r="E11" s="71"/>
-      <c r="F11" s="86"/>
+      <c r="F11" s="97"/>
       <c r="G11" s="71"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="99"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="112"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
     </row>
-    <row r="12" spans="1:24" ht="12" customHeight="1">
+    <row r="12" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
@@ -1793,57 +1817,57 @@
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
     </row>
-    <row r="13" spans="1:24" ht="55.5" customHeight="1">
-      <c r="A13" s="85" t="s">
+    <row r="13" spans="1:24" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="96" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="75" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="77" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="74" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="69" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="86" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="76"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
     </row>
-    <row r="14" spans="1:24" ht="46.5" customHeight="1">
-      <c r="A14" s="85"/>
-      <c r="B14" s="69" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="77" t="s">
+    <row r="14" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="96"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="76" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="71"/>
       <c r="E14" s="69" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="86"/>
+        <v>69</v>
+      </c>
+      <c r="F14" s="97"/>
       <c r="G14" s="69" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" s="87"/>
-      <c r="I14" s="87"/>
+        <v>71</v>
+      </c>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
       <c r="J14" s="27"/>
       <c r="K14" s="27"/>
     </row>
-    <row r="15" spans="1:24" ht="12" customHeight="1">
+    <row r="15" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="29"/>
       <c r="C15" s="30"/>
@@ -1856,67 +1880,67 @@
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
     </row>
-    <row r="16" spans="1:24" ht="63.75" customHeight="1">
-      <c r="A16" s="88" t="s">
+    <row r="16" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="108" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="109"/>
+      <c r="D16" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="E16" s="77" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="78" t="s">
+      <c r="E16" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="69"/>
+      <c r="G16" s="91" t="s">
+        <v>104</v>
+      </c>
       <c r="H16" s="70"/>
-      <c r="I16" s="77"/>
+      <c r="I16" s="76"/>
       <c r="J16" s="27"/>
       <c r="K16" s="27"/>
     </row>
-    <row r="17" spans="1:11" ht="63.75" customHeight="1">
-      <c r="A17" s="89"/>
-      <c r="B17" s="97" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="97"/>
+    <row r="17" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="100"/>
+      <c r="B17" s="110" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="110"/>
       <c r="D17" s="70"/>
-      <c r="E17" s="74" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="78"/>
-      <c r="G17" s="91" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" s="92"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="102" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" s="103"/>
       <c r="I17" s="69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J17" s="27"/>
       <c r="K17" s="27"/>
     </row>
-    <row r="18" spans="1:11" ht="75.75" customHeight="1">
-      <c r="A18" s="90"/>
-      <c r="B18" s="79"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="78" t="s">
+    <row r="18" spans="1:11" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="101"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="91" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="92"/>
-      <c r="I18" s="81"/>
+      <c r="G18" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="105"/>
+      <c r="I18" s="80"/>
       <c r="K18" s="27"/>
     </row>
-    <row r="19" spans="1:11" ht="12" customHeight="1">
+    <row r="19" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="29"/>
       <c r="C19" s="30"/>
@@ -1929,12 +1953,12 @@
       <c r="J19" s="27"/>
       <c r="K19" s="27"/>
     </row>
-    <row r="20" spans="1:11" ht="53.25" customHeight="1">
-      <c r="A20" s="88" t="s">
+    <row r="20" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="99" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="69" t="s">
         <v>68</v>
@@ -1948,16 +1972,16 @@
       <c r="J20" s="27"/>
       <c r="K20" s="27"/>
     </row>
-    <row r="21" spans="1:11" ht="56.25" customHeight="1">
-      <c r="A21" s="90"/>
+    <row r="21" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="101"/>
       <c r="B21" s="69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
+        <v>99</v>
+      </c>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
       <c r="F21" s="34"/>
       <c r="G21" s="32"/>
       <c r="H21" s="5"/>
@@ -1965,7 +1989,7 @@
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
     </row>
-    <row r="22" spans="1:11" ht="12" customHeight="1">
+    <row r="22" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="29"/>
       <c r="C22" s="30"/>
@@ -1978,7 +2002,7 @@
       <c r="J22" s="27"/>
       <c r="K22" s="27"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" s="36" t="s">
         <v>16</v>
@@ -1996,19 +2020,19 @@
       <c r="G23" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="102" t="s">
+      <c r="H23" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="102"/>
+      <c r="I23" s="115"/>
       <c r="J23" s="27"/>
       <c r="K23" s="27"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="42"/>
-      <c r="B24" s="109" t="s">
+      <c r="B24" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="109" t="s">
+      <c r="C24" s="83" t="s">
         <v>50</v>
       </c>
       <c r="D24" s="25"/>
@@ -2017,19 +2041,19 @@
       <c r="G24" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="103" t="s">
+      <c r="H24" s="93" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="103"/>
+      <c r="I24" s="93"/>
       <c r="J24" s="27"/>
       <c r="K24" s="27"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="42"/>
-      <c r="B25" s="110" t="s">
+      <c r="B25" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="109" t="s">
+      <c r="C25" s="83" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="25"/>
@@ -2038,183 +2062,183 @@
       <c r="G25" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="103" t="s">
+      <c r="H25" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="103"/>
+      <c r="I25" s="93"/>
       <c r="J25" s="27"/>
       <c r="K25" s="27"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="42"/>
-      <c r="B26" s="110" t="s">
+      <c r="B26" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="109" t="s">
+      <c r="C26" s="83" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26" s="43"/>
       <c r="F26" s="44"/>
-      <c r="G26" s="111"/>
-      <c r="H26" s="112" t="s">
+      <c r="G26" s="85"/>
+      <c r="H26" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="112"/>
+      <c r="I26" s="95"/>
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="42"/>
-      <c r="B27" s="110" t="s">
+      <c r="B27" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="109" t="s">
+      <c r="C27" s="83" t="s">
         <v>56</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="43"/>
       <c r="F27" s="44"/>
-      <c r="G27" s="113" t="s">
+      <c r="G27" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="114" t="s">
+      <c r="H27" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="114"/>
+      <c r="I27" s="87"/>
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="42"/>
-      <c r="B28" s="110" t="s">
+      <c r="B28" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="109" t="s">
+      <c r="C28" s="83" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="45"/>
       <c r="F28" s="46"/>
-      <c r="G28" s="113" t="s">
+      <c r="G28" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="H28" s="114" t="s">
+      <c r="H28" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="I28" s="114"/>
+      <c r="I28" s="87"/>
       <c r="J28" s="27"/>
       <c r="K28" s="27"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="42"/>
-      <c r="B29" s="110" t="s">
+      <c r="B29" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="83" t="s">
         <v>81</v>
-      </c>
-      <c r="C29" s="109" t="s">
-        <v>83</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="45"/>
       <c r="F29" s="46"/>
-      <c r="G29" s="111"/>
-      <c r="H29" s="112" t="s">
+      <c r="G29" s="85"/>
+      <c r="H29" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="I29" s="112"/>
+      <c r="I29" s="95"/>
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="42"/>
-      <c r="B30" s="110" t="s">
+      <c r="B30" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="109" t="s">
+      <c r="C30" s="83" t="s">
         <v>60</v>
       </c>
       <c r="D30" s="66"/>
       <c r="E30" s="45"/>
       <c r="F30" s="46"/>
-      <c r="G30" s="113" t="s">
+      <c r="G30" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="113" t="s">
+      <c r="H30" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="115"/>
+      <c r="I30" s="88"/>
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="42"/>
-      <c r="B31" s="110" t="s">
+      <c r="B31" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="109" t="s">
+      <c r="C31" s="83" t="s">
         <v>61</v>
       </c>
       <c r="D31" s="66"/>
       <c r="E31" s="45"/>
       <c r="F31" s="46"/>
-      <c r="G31" s="113" t="s">
+      <c r="G31" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="H31" s="113" t="s">
+      <c r="H31" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="I31" s="116"/>
+      <c r="I31" s="89"/>
       <c r="J31" s="27"/>
       <c r="K31" s="27"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="42"/>
-      <c r="B32" s="110" t="s">
+      <c r="B32" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="109" t="s">
+      <c r="C32" s="83" t="s">
         <v>63</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="45"/>
       <c r="F32" s="46"/>
-      <c r="G32" s="117" t="s">
+      <c r="G32" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="103" t="s">
+      <c r="H32" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="I32" s="103"/>
+      <c r="I32" s="93"/>
       <c r="J32" s="27"/>
       <c r="K32" s="27"/>
     </row>
-    <row r="33" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
+    <row r="33" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="47"/>
-      <c r="B33" s="110" t="s">
+      <c r="B33" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="110" t="s">
+      <c r="C33" s="84" t="s">
         <v>64</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="45"/>
       <c r="F33" s="46"/>
-      <c r="G33" s="117" t="s">
+      <c r="G33" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="H33" s="103" t="s">
+      <c r="H33" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="103"/>
+      <c r="I33" s="93"/>
       <c r="J33" s="27"/>
       <c r="K33" s="27"/>
     </row>
-    <row r="34" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
+    <row r="34" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="48"/>
-      <c r="B34" s="110" t="s">
+      <c r="B34" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="110" t="s">
+      <c r="C34" s="84" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="25"/>
@@ -2223,20 +2247,20 @@
       <c r="G34" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H34" s="103" t="s">
+      <c r="H34" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="I34" s="103"/>
+      <c r="I34" s="93"/>
       <c r="J34" s="27"/>
       <c r="K34" s="27"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="48"/>
-      <c r="B35" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="110" t="s">
-        <v>92</v>
+      <c r="B35" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="84" t="s">
+        <v>87</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="45"/>
@@ -2244,20 +2268,20 @@
       <c r="G35" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="H35" s="103" t="s">
+      <c r="H35" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I35" s="103"/>
+      <c r="I35" s="93"/>
       <c r="J35" s="27"/>
       <c r="K35" s="27"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="48"/>
-      <c r="B36" s="110" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="110" t="s">
-        <v>94</v>
+      <c r="B36" s="84" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="84" t="s">
+        <v>89</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="45"/>
@@ -2266,7 +2290,7 @@
       <c r="H36" s="45"/>
       <c r="I36" s="45"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
       <c r="B37" s="65"/>
       <c r="C37" s="26"/>
@@ -2277,7 +2301,7 @@
       <c r="H37" s="52"/>
       <c r="I37" s="52"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="53"/>
       <c r="D38" s="54"/>
       <c r="E38" s="17"/>
@@ -2286,13 +2310,13 @@
       <c r="H38" s="56"/>
       <c r="I38" s="56"/>
       <c r="J38" s="6"/>
-      <c r="Q38" s="82" t="s">
+      <c r="Q38" s="81" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A39" s="84"/>
-      <c r="B39" s="84"/>
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="94"/>
+      <c r="B39" s="94"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2307,7 +2331,7 @@
       <c r="N39" s="13"/>
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
-      <c r="Q39" s="83" t="s">
+      <c r="Q39" s="82" t="s">
         <v>39</v>
       </c>
       <c r="R39" s="13"/>
@@ -2318,7 +2342,7 @@
       <c r="W39" s="13"/>
       <c r="X39" s="13"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="12"/>
       <c r="C40" s="11"/>
@@ -2344,7 +2368,7 @@
       <c r="W40" s="13"/>
       <c r="X40" s="13"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="12"/>
       <c r="C41" s="11"/>
@@ -2370,7 +2394,7 @@
       <c r="W41" s="13"/>
       <c r="X41" s="13"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -2396,7 +2420,7 @@
       <c r="W42" s="13"/>
       <c r="X42" s="13"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -2422,7 +2446,7 @@
       <c r="W43" s="13"/>
       <c r="X43" s="13"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="53"/>
       <c r="B44" s="58"/>
       <c r="C44" s="17"/>
@@ -2448,7 +2472,7 @@
       <c r="W44" s="13"/>
       <c r="X44" s="13"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="53"/>
       <c r="B45" s="58"/>
       <c r="C45" s="17"/>
@@ -2474,7 +2498,7 @@
       <c r="W45" s="13"/>
       <c r="X45" s="13"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="53"/>
       <c r="B46" s="58"/>
       <c r="C46" s="17"/>
@@ -2500,7 +2524,7 @@
       <c r="W46" s="13"/>
       <c r="X46" s="13"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="53"/>
       <c r="B47" s="58"/>
       <c r="C47" s="17"/>
@@ -2526,7 +2550,7 @@
       <c r="W47" s="13"/>
       <c r="X47" s="13"/>
     </row>
-    <row r="48" spans="1:24" ht="15.75" customHeight="1">
+    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="53"/>
       <c r="B48" s="58"/>
       <c r="C48" s="17"/>
@@ -2538,7 +2562,7 @@
       <c r="I48" s="54"/>
       <c r="J48" s="6"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75" customHeight="1">
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="53"/>
       <c r="B49" s="58"/>
       <c r="C49" s="17"/>
@@ -2549,1529 +2573,1529 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75" customHeight="1">
+    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18"/>
       <c r="F50" s="63"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" customHeight="1">
+    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
       <c r="F51" s="63"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75" customHeight="1">
+    <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="F52" s="63"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75" customHeight="1">
+    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
       <c r="F53" s="63"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75" customHeight="1">
+    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
       <c r="F54" s="63"/>
     </row>
-    <row r="55" spans="1:9" ht="15.75" customHeight="1">
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18"/>
       <c r="F55" s="63"/>
     </row>
-    <row r="56" spans="1:9" ht="15.75" customHeight="1">
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
       <c r="F56" s="63"/>
     </row>
-    <row r="57" spans="1:9" ht="15.75" customHeight="1">
+    <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="18"/>
       <c r="F57" s="63"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75" customHeight="1">
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18"/>
       <c r="F58" s="63"/>
     </row>
-    <row r="59" spans="1:9" ht="15.75" customHeight="1">
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="F59" s="63"/>
     </row>
-    <row r="60" spans="1:9" ht="15.75" customHeight="1">
+    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
       <c r="F60" s="63"/>
     </row>
-    <row r="61" spans="1:9" ht="15.75" customHeight="1">
+    <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
       <c r="F61" s="63"/>
     </row>
-    <row r="62" spans="1:9" ht="15.75" customHeight="1">
+    <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="F62" s="63"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75" customHeight="1">
+    <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="F63" s="63"/>
     </row>
-    <row r="64" spans="1:9" ht="15.75" customHeight="1">
+    <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18"/>
       <c r="F64" s="63"/>
     </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1">
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
       <c r="F65" s="63"/>
     </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1">
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18"/>
       <c r="F66" s="63"/>
     </row>
-    <row r="67" spans="1:6" ht="15.75" customHeight="1">
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18"/>
       <c r="F67" s="63"/>
     </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1">
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18"/>
       <c r="F68" s="63"/>
     </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1">
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18"/>
       <c r="F69" s="63"/>
     </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1">
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="18"/>
       <c r="F70" s="63"/>
     </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1">
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="F71" s="63"/>
     </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1">
+    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="F72" s="63"/>
     </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1">
+    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="F73" s="63"/>
     </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1">
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="18"/>
       <c r="F74" s="63"/>
     </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1">
+    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="18"/>
       <c r="F75" s="63"/>
     </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1">
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="18"/>
       <c r="F76" s="63"/>
     </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1">
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="18"/>
       <c r="F77" s="63"/>
     </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1">
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="18"/>
       <c r="F78" s="63"/>
     </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1">
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18"/>
       <c r="F79" s="63"/>
     </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1">
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="18"/>
       <c r="F80" s="63"/>
     </row>
-    <row r="81" spans="1:6" ht="15.75" customHeight="1">
+    <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="18"/>
       <c r="F81" s="63"/>
     </row>
-    <row r="82" spans="1:6" ht="15.75" customHeight="1">
+    <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="18"/>
       <c r="F82" s="63"/>
     </row>
-    <row r="83" spans="1:6" ht="15.75" customHeight="1">
+    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="18"/>
       <c r="F83" s="63"/>
     </row>
-    <row r="84" spans="1:6" ht="15.75" customHeight="1">
+    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="18"/>
       <c r="F84" s="63"/>
     </row>
-    <row r="85" spans="1:6" ht="15.75" customHeight="1">
+    <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="18"/>
       <c r="F85" s="63"/>
     </row>
-    <row r="86" spans="1:6" ht="15.75" customHeight="1">
+    <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="18"/>
       <c r="F86" s="63"/>
     </row>
-    <row r="87" spans="1:6" ht="15.75" customHeight="1">
+    <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="18"/>
       <c r="F87" s="63"/>
     </row>
-    <row r="88" spans="1:6" ht="15.75" customHeight="1">
+    <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="18"/>
       <c r="F88" s="63"/>
     </row>
-    <row r="89" spans="1:6" ht="15.75" customHeight="1">
+    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="18"/>
       <c r="F89" s="63"/>
     </row>
-    <row r="90" spans="1:6" ht="15.75" customHeight="1">
+    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="18"/>
       <c r="F90" s="63"/>
     </row>
-    <row r="91" spans="1:6" ht="15.75" customHeight="1">
+    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="18"/>
       <c r="F91" s="63"/>
     </row>
-    <row r="92" spans="1:6" ht="15.75" customHeight="1">
+    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="18"/>
       <c r="F92" s="63"/>
     </row>
-    <row r="93" spans="1:6" ht="15.75" customHeight="1">
+    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="18"/>
       <c r="F93" s="63"/>
     </row>
-    <row r="94" spans="1:6" ht="15.75" customHeight="1">
+    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="18"/>
       <c r="F94" s="63"/>
     </row>
-    <row r="95" spans="1:6" ht="15.75" customHeight="1">
+    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="18"/>
       <c r="F95" s="63"/>
     </row>
-    <row r="96" spans="1:6" ht="15.75" customHeight="1">
+    <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="18"/>
       <c r="F96" s="63"/>
     </row>
-    <row r="97" spans="1:6" ht="15.75" customHeight="1">
+    <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="18"/>
       <c r="F97" s="63"/>
     </row>
-    <row r="98" spans="1:6" ht="15.75" customHeight="1">
+    <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="18"/>
       <c r="F98" s="63"/>
     </row>
-    <row r="99" spans="1:6" ht="15.75" customHeight="1">
+    <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="18"/>
       <c r="F99" s="63"/>
     </row>
-    <row r="100" spans="1:6" ht="15.75" customHeight="1">
+    <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="18"/>
       <c r="F100" s="63"/>
     </row>
-    <row r="101" spans="1:6" ht="15.75" customHeight="1">
+    <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="18"/>
       <c r="F101" s="63"/>
     </row>
-    <row r="102" spans="1:6" ht="15.75" customHeight="1">
+    <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="18"/>
       <c r="F102" s="63"/>
     </row>
-    <row r="103" spans="1:6" ht="15.75" customHeight="1">
+    <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="18"/>
       <c r="F103" s="63"/>
     </row>
-    <row r="104" spans="1:6" ht="15.75" customHeight="1">
+    <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="18"/>
       <c r="F104" s="63"/>
     </row>
-    <row r="105" spans="1:6" ht="15.75" customHeight="1">
+    <row r="105" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="18"/>
       <c r="F105" s="63"/>
     </row>
-    <row r="106" spans="1:6" ht="15.75" customHeight="1">
+    <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="18"/>
       <c r="F106" s="63"/>
     </row>
-    <row r="107" spans="1:6" ht="15.75" customHeight="1">
+    <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="18"/>
       <c r="F107" s="63"/>
     </row>
-    <row r="108" spans="1:6" ht="15.75" customHeight="1">
+    <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="18"/>
       <c r="F108" s="63"/>
     </row>
-    <row r="109" spans="1:6" ht="15.75" customHeight="1">
+    <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="18"/>
       <c r="F109" s="63"/>
     </row>
-    <row r="110" spans="1:6" ht="15.75" customHeight="1">
+    <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="18"/>
       <c r="F110" s="63"/>
     </row>
-    <row r="111" spans="1:6" ht="15.75" customHeight="1">
+    <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="18"/>
       <c r="F111" s="63"/>
     </row>
-    <row r="112" spans="1:6" ht="15.75" customHeight="1">
+    <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="18"/>
       <c r="F112" s="63"/>
     </row>
-    <row r="113" spans="1:6" ht="15.75" customHeight="1">
+    <row r="113" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="18"/>
       <c r="F113" s="63"/>
     </row>
-    <row r="114" spans="1:6" ht="15.75" customHeight="1">
+    <row r="114" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="18"/>
       <c r="F114" s="63"/>
     </row>
-    <row r="115" spans="1:6" ht="15.75" customHeight="1">
+    <row r="115" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="18"/>
       <c r="F115" s="63"/>
     </row>
-    <row r="116" spans="1:6" ht="15.75" customHeight="1">
+    <row r="116" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="18"/>
       <c r="F116" s="63"/>
     </row>
-    <row r="117" spans="1:6" ht="15.75" customHeight="1">
+    <row r="117" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="18"/>
       <c r="F117" s="63"/>
     </row>
-    <row r="118" spans="1:6" ht="15.75" customHeight="1">
+    <row r="118" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="18"/>
       <c r="F118" s="63"/>
     </row>
-    <row r="119" spans="1:6" ht="15.75" customHeight="1">
+    <row r="119" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="18"/>
       <c r="F119" s="63"/>
     </row>
-    <row r="120" spans="1:6" ht="15.75" customHeight="1">
+    <row r="120" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="18"/>
       <c r="F120" s="63"/>
     </row>
-    <row r="121" spans="1:6" ht="15.75" customHeight="1">
+    <row r="121" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="18"/>
       <c r="F121" s="63"/>
     </row>
-    <row r="122" spans="1:6" ht="15.75" customHeight="1">
+    <row r="122" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="18"/>
       <c r="F122" s="63"/>
     </row>
-    <row r="123" spans="1:6" ht="15.75" customHeight="1">
+    <row r="123" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="18"/>
       <c r="F123" s="63"/>
     </row>
-    <row r="124" spans="1:6" ht="15.75" customHeight="1">
+    <row r="124" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="18"/>
       <c r="F124" s="63"/>
     </row>
-    <row r="125" spans="1:6" ht="15.75" customHeight="1">
+    <row r="125" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="18"/>
       <c r="F125" s="63"/>
     </row>
-    <row r="126" spans="1:6" ht="15.75" customHeight="1">
+    <row r="126" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="18"/>
       <c r="F126" s="63"/>
     </row>
-    <row r="127" spans="1:6" ht="15.75" customHeight="1">
+    <row r="127" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="18"/>
       <c r="F127" s="63"/>
     </row>
-    <row r="128" spans="1:6" ht="15.75" customHeight="1">
+    <row r="128" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="18"/>
       <c r="F128" s="63"/>
     </row>
-    <row r="129" spans="1:6" ht="15.75" customHeight="1">
+    <row r="129" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="18"/>
       <c r="F129" s="63"/>
     </row>
-    <row r="130" spans="1:6" ht="15.75" customHeight="1">
+    <row r="130" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="18"/>
       <c r="F130" s="63"/>
     </row>
-    <row r="131" spans="1:6" ht="15.75" customHeight="1">
+    <row r="131" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="18"/>
       <c r="F131" s="63"/>
     </row>
-    <row r="132" spans="1:6" ht="15.75" customHeight="1">
+    <row r="132" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="18"/>
       <c r="F132" s="63"/>
     </row>
-    <row r="133" spans="1:6" ht="15.75" customHeight="1">
+    <row r="133" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="18"/>
       <c r="F133" s="63"/>
     </row>
-    <row r="134" spans="1:6" ht="15.75" customHeight="1">
+    <row r="134" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="18"/>
       <c r="F134" s="63"/>
     </row>
-    <row r="135" spans="1:6" ht="15.75" customHeight="1">
+    <row r="135" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="18"/>
       <c r="F135" s="63"/>
     </row>
-    <row r="136" spans="1:6" ht="15.75" customHeight="1">
+    <row r="136" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="18"/>
       <c r="F136" s="63"/>
     </row>
-    <row r="137" spans="1:6" ht="15.75" customHeight="1">
+    <row r="137" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="18"/>
       <c r="F137" s="63"/>
     </row>
-    <row r="138" spans="1:6" ht="15.75" customHeight="1">
+    <row r="138" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="18"/>
       <c r="F138" s="63"/>
     </row>
-    <row r="139" spans="1:6" ht="15.75" customHeight="1">
+    <row r="139" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="18"/>
       <c r="F139" s="63"/>
     </row>
-    <row r="140" spans="1:6" ht="15.75" customHeight="1">
+    <row r="140" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="18"/>
       <c r="F140" s="63"/>
     </row>
-    <row r="141" spans="1:6" ht="15.75" customHeight="1">
+    <row r="141" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="18"/>
       <c r="F141" s="63"/>
     </row>
-    <row r="142" spans="1:6" ht="15.75" customHeight="1">
+    <row r="142" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="18"/>
       <c r="F142" s="63"/>
     </row>
-    <row r="143" spans="1:6" ht="15.75" customHeight="1">
+    <row r="143" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="18"/>
       <c r="F143" s="63"/>
     </row>
-    <row r="144" spans="1:6" ht="15.75" customHeight="1">
+    <row r="144" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="18"/>
       <c r="F144" s="63"/>
     </row>
-    <row r="145" spans="1:6" ht="15.75" customHeight="1">
+    <row r="145" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="18"/>
       <c r="F145" s="63"/>
     </row>
-    <row r="146" spans="1:6" ht="15.75" customHeight="1">
+    <row r="146" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="18"/>
       <c r="F146" s="63"/>
     </row>
-    <row r="147" spans="1:6" ht="15.75" customHeight="1">
+    <row r="147" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="18"/>
       <c r="F147" s="63"/>
     </row>
-    <row r="148" spans="1:6" ht="15.75" customHeight="1">
+    <row r="148" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="18"/>
       <c r="F148" s="63"/>
     </row>
-    <row r="149" spans="1:6" ht="15.75" customHeight="1">
+    <row r="149" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="18"/>
       <c r="F149" s="63"/>
     </row>
-    <row r="150" spans="1:6" ht="15.75" customHeight="1">
+    <row r="150" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="18"/>
       <c r="F150" s="63"/>
     </row>
-    <row r="151" spans="1:6" ht="15.75" customHeight="1">
+    <row r="151" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="18"/>
       <c r="F151" s="63"/>
     </row>
-    <row r="152" spans="1:6" ht="15.75" customHeight="1">
+    <row r="152" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="18"/>
       <c r="F152" s="63"/>
     </row>
-    <row r="153" spans="1:6" ht="15.75" customHeight="1">
+    <row r="153" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="18"/>
       <c r="F153" s="63"/>
     </row>
-    <row r="154" spans="1:6" ht="15.75" customHeight="1">
+    <row r="154" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="18"/>
       <c r="F154" s="63"/>
     </row>
-    <row r="155" spans="1:6" ht="15.75" customHeight="1">
+    <row r="155" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="18"/>
       <c r="F155" s="63"/>
     </row>
-    <row r="156" spans="1:6" ht="15.75" customHeight="1">
+    <row r="156" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="18"/>
       <c r="F156" s="63"/>
     </row>
-    <row r="157" spans="1:6" ht="15.75" customHeight="1">
+    <row r="157" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="18"/>
       <c r="F157" s="63"/>
     </row>
-    <row r="158" spans="1:6" ht="15.75" customHeight="1">
+    <row r="158" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="18"/>
       <c r="F158" s="63"/>
     </row>
-    <row r="159" spans="1:6" ht="15.75" customHeight="1">
+    <row r="159" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="18"/>
       <c r="F159" s="63"/>
     </row>
-    <row r="160" spans="1:6" ht="15.75" customHeight="1">
+    <row r="160" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="18"/>
       <c r="F160" s="63"/>
     </row>
-    <row r="161" spans="1:6" ht="15.75" customHeight="1">
+    <row r="161" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="18"/>
       <c r="F161" s="63"/>
     </row>
-    <row r="162" spans="1:6" ht="15.75" customHeight="1">
+    <row r="162" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="18"/>
       <c r="F162" s="63"/>
     </row>
-    <row r="163" spans="1:6" ht="15.75" customHeight="1">
+    <row r="163" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="18"/>
       <c r="F163" s="63"/>
     </row>
-    <row r="164" spans="1:6" ht="15.75" customHeight="1">
+    <row r="164" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="18"/>
       <c r="F164" s="63"/>
     </row>
-    <row r="165" spans="1:6" ht="15.75" customHeight="1">
+    <row r="165" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="18"/>
       <c r="F165" s="63"/>
     </row>
-    <row r="166" spans="1:6" ht="15.75" customHeight="1">
+    <row r="166" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="18"/>
       <c r="F166" s="63"/>
     </row>
-    <row r="167" spans="1:6" ht="15.75" customHeight="1">
+    <row r="167" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="18"/>
       <c r="F167" s="63"/>
     </row>
-    <row r="168" spans="1:6" ht="15.75" customHeight="1">
+    <row r="168" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="18"/>
       <c r="F168" s="63"/>
     </row>
-    <row r="169" spans="1:6" ht="15.75" customHeight="1">
+    <row r="169" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="18"/>
       <c r="F169" s="63"/>
     </row>
-    <row r="170" spans="1:6" ht="15.75" customHeight="1">
+    <row r="170" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="18"/>
       <c r="F170" s="63"/>
     </row>
-    <row r="171" spans="1:6" ht="15.75" customHeight="1">
+    <row r="171" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="18"/>
       <c r="F171" s="63"/>
     </row>
-    <row r="172" spans="1:6" ht="15.75" customHeight="1">
+    <row r="172" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="18"/>
       <c r="F172" s="63"/>
     </row>
-    <row r="173" spans="1:6" ht="15.75" customHeight="1">
+    <row r="173" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="18"/>
       <c r="F173" s="63"/>
     </row>
-    <row r="174" spans="1:6" ht="15.75" customHeight="1">
+    <row r="174" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="18"/>
       <c r="F174" s="63"/>
     </row>
-    <row r="175" spans="1:6" ht="15.75" customHeight="1">
+    <row r="175" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="18"/>
       <c r="F175" s="63"/>
     </row>
-    <row r="176" spans="1:6" ht="15.75" customHeight="1">
+    <row r="176" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="18"/>
       <c r="F176" s="63"/>
     </row>
-    <row r="177" spans="1:6" ht="15.75" customHeight="1">
+    <row r="177" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="18"/>
       <c r="F177" s="63"/>
     </row>
-    <row r="178" spans="1:6" ht="15.75" customHeight="1">
+    <row r="178" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="18"/>
       <c r="F178" s="63"/>
     </row>
-    <row r="179" spans="1:6" ht="15.75" customHeight="1">
+    <row r="179" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="18"/>
       <c r="F179" s="63"/>
     </row>
-    <row r="180" spans="1:6" ht="15.75" customHeight="1">
+    <row r="180" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="18"/>
       <c r="F180" s="63"/>
     </row>
-    <row r="181" spans="1:6" ht="15.75" customHeight="1">
+    <row r="181" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="18"/>
       <c r="F181" s="63"/>
     </row>
-    <row r="182" spans="1:6" ht="15.75" customHeight="1">
+    <row r="182" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="18"/>
       <c r="F182" s="63"/>
     </row>
-    <row r="183" spans="1:6" ht="15.75" customHeight="1">
+    <row r="183" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="18"/>
       <c r="F183" s="63"/>
     </row>
-    <row r="184" spans="1:6" ht="15.75" customHeight="1">
+    <row r="184" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="18"/>
       <c r="F184" s="63"/>
     </row>
-    <row r="185" spans="1:6" ht="15.75" customHeight="1">
+    <row r="185" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="18"/>
       <c r="F185" s="63"/>
     </row>
-    <row r="186" spans="1:6" ht="15.75" customHeight="1">
+    <row r="186" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="18"/>
       <c r="F186" s="63"/>
     </row>
-    <row r="187" spans="1:6" ht="15.75" customHeight="1">
+    <row r="187" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="18"/>
       <c r="F187" s="63"/>
     </row>
-    <row r="188" spans="1:6" ht="15.75" customHeight="1">
+    <row r="188" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="18"/>
       <c r="F188" s="63"/>
     </row>
-    <row r="189" spans="1:6" ht="15.75" customHeight="1">
+    <row r="189" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="18"/>
       <c r="F189" s="63"/>
     </row>
-    <row r="190" spans="1:6" ht="15.75" customHeight="1">
+    <row r="190" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="18"/>
       <c r="F190" s="63"/>
     </row>
-    <row r="191" spans="1:6" ht="15.75" customHeight="1">
+    <row r="191" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="18"/>
       <c r="F191" s="63"/>
     </row>
-    <row r="192" spans="1:6" ht="15.75" customHeight="1">
+    <row r="192" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="18"/>
       <c r="F192" s="63"/>
     </row>
-    <row r="193" spans="1:6" ht="15.75" customHeight="1">
+    <row r="193" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="18"/>
       <c r="F193" s="63"/>
     </row>
-    <row r="194" spans="1:6" ht="15.75" customHeight="1">
+    <row r="194" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="18"/>
       <c r="F194" s="63"/>
     </row>
-    <row r="195" spans="1:6" ht="15.75" customHeight="1">
+    <row r="195" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="18"/>
       <c r="F195" s="63"/>
     </row>
-    <row r="196" spans="1:6" ht="15.75" customHeight="1">
+    <row r="196" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="18"/>
       <c r="F196" s="63"/>
     </row>
-    <row r="197" spans="1:6" ht="15.75" customHeight="1">
+    <row r="197" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="18"/>
       <c r="F197" s="63"/>
     </row>
-    <row r="198" spans="1:6" ht="15.75" customHeight="1">
+    <row r="198" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="18"/>
       <c r="F198" s="63"/>
     </row>
-    <row r="199" spans="1:6" ht="15.75" customHeight="1">
+    <row r="199" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="18"/>
       <c r="F199" s="63"/>
     </row>
-    <row r="200" spans="1:6" ht="15.75" customHeight="1">
+    <row r="200" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="18"/>
       <c r="F200" s="63"/>
     </row>
-    <row r="201" spans="1:6" ht="15.75" customHeight="1">
+    <row r="201" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="18"/>
       <c r="F201" s="63"/>
     </row>
-    <row r="202" spans="1:6" ht="15.75" customHeight="1">
+    <row r="202" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="18"/>
       <c r="F202" s="63"/>
     </row>
-    <row r="203" spans="1:6" ht="15.75" customHeight="1">
+    <row r="203" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="18"/>
       <c r="F203" s="63"/>
     </row>
-    <row r="204" spans="1:6" ht="15.75" customHeight="1">
+    <row r="204" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="18"/>
       <c r="F204" s="63"/>
     </row>
-    <row r="205" spans="1:6" ht="15.75" customHeight="1">
+    <row r="205" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="18"/>
       <c r="F205" s="63"/>
     </row>
-    <row r="206" spans="1:6" ht="15.75" customHeight="1">
+    <row r="206" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="18"/>
       <c r="F206" s="63"/>
     </row>
-    <row r="207" spans="1:6" ht="15.75" customHeight="1">
+    <row r="207" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="18"/>
       <c r="F207" s="63"/>
     </row>
-    <row r="208" spans="1:6" ht="15.75" customHeight="1">
+    <row r="208" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="18"/>
       <c r="F208" s="63"/>
     </row>
-    <row r="209" spans="1:6" ht="15.75" customHeight="1">
+    <row r="209" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="18"/>
       <c r="F209" s="63"/>
     </row>
-    <row r="210" spans="1:6" ht="15.75" customHeight="1">
+    <row r="210" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="18"/>
       <c r="F210" s="63"/>
     </row>
-    <row r="211" spans="1:6" ht="15.75" customHeight="1">
+    <row r="211" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="18"/>
       <c r="F211" s="63"/>
     </row>
-    <row r="212" spans="1:6" ht="15.75" customHeight="1">
+    <row r="212" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="18"/>
       <c r="F212" s="63"/>
     </row>
-    <row r="213" spans="1:6" ht="15.75" customHeight="1">
+    <row r="213" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="18"/>
       <c r="F213" s="63"/>
     </row>
-    <row r="214" spans="1:6" ht="15.75" customHeight="1">
+    <row r="214" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="18"/>
       <c r="F214" s="63"/>
     </row>
-    <row r="215" spans="1:6" ht="15.75" customHeight="1">
+    <row r="215" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="18"/>
       <c r="F215" s="63"/>
     </row>
-    <row r="216" spans="1:6" ht="15.75" customHeight="1">
+    <row r="216" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="18"/>
       <c r="F216" s="63"/>
     </row>
-    <row r="217" spans="1:6" ht="15.75" customHeight="1">
+    <row r="217" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="18"/>
       <c r="F217" s="63"/>
     </row>
-    <row r="218" spans="1:6" ht="15.75" customHeight="1">
+    <row r="218" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="18"/>
       <c r="F218" s="63"/>
     </row>
-    <row r="219" spans="1:6" ht="15.75" customHeight="1">
+    <row r="219" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="18"/>
       <c r="F219" s="63"/>
     </row>
-    <row r="220" spans="1:6" ht="15.75" customHeight="1">
+    <row r="220" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="18"/>
       <c r="F220" s="63"/>
     </row>
-    <row r="221" spans="1:6" ht="15.75" customHeight="1">
+    <row r="221" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="18"/>
       <c r="F221" s="63"/>
     </row>
-    <row r="222" spans="1:6" ht="15.75" customHeight="1">
+    <row r="222" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="18"/>
       <c r="F222" s="63"/>
     </row>
-    <row r="223" spans="1:6" ht="15.75" customHeight="1">
+    <row r="223" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="18"/>
       <c r="F223" s="63"/>
     </row>
-    <row r="224" spans="1:6" ht="15.75" customHeight="1">
+    <row r="224" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="18"/>
       <c r="F224" s="63"/>
     </row>
-    <row r="225" spans="1:6" ht="15.75" customHeight="1">
+    <row r="225" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="18"/>
       <c r="F225" s="63"/>
     </row>
-    <row r="226" spans="1:6" ht="15.75" customHeight="1">
+    <row r="226" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="18"/>
       <c r="F226" s="63"/>
     </row>
-    <row r="227" spans="1:6" ht="15.75" customHeight="1">
+    <row r="227" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="18"/>
       <c r="F227" s="63"/>
     </row>
-    <row r="228" spans="1:6" ht="15.75" customHeight="1">
+    <row r="228" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="18"/>
       <c r="F228" s="63"/>
     </row>
-    <row r="229" spans="1:6" ht="15.75" customHeight="1">
+    <row r="229" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="18"/>
       <c r="F229" s="63"/>
     </row>
-    <row r="230" spans="1:6" ht="15.75" customHeight="1">
+    <row r="230" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="18"/>
       <c r="F230" s="63"/>
     </row>
-    <row r="231" spans="1:6" ht="15.75" customHeight="1">
+    <row r="231" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="18"/>
       <c r="F231" s="63"/>
     </row>
-    <row r="232" spans="1:6" ht="15.75" customHeight="1">
+    <row r="232" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="18"/>
       <c r="F232" s="63"/>
     </row>
-    <row r="233" spans="1:6" ht="15.75" customHeight="1">
+    <row r="233" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="18"/>
       <c r="F233" s="63"/>
     </row>
-    <row r="234" spans="1:6" ht="15.75" customHeight="1">
+    <row r="234" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="18"/>
       <c r="F234" s="63"/>
     </row>
-    <row r="235" spans="1:6" ht="15.75" customHeight="1">
+    <row r="235" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="18"/>
       <c r="F235" s="63"/>
     </row>
-    <row r="236" spans="1:6" ht="15.75" customHeight="1">
+    <row r="236" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="18"/>
       <c r="F236" s="63"/>
     </row>
-    <row r="237" spans="1:6" ht="15.75" customHeight="1">
+    <row r="237" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="18"/>
       <c r="F237" s="63"/>
     </row>
-    <row r="238" spans="1:6" ht="15.75" customHeight="1">
+    <row r="238" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="18"/>
       <c r="F238" s="63"/>
     </row>
-    <row r="239" spans="1:6" ht="15.75" customHeight="1">
+    <row r="239" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="18"/>
       <c r="F239" s="63"/>
     </row>
-    <row r="240" spans="1:6" ht="15.75" customHeight="1">
+    <row r="240" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="18"/>
       <c r="F240" s="63"/>
     </row>
-    <row r="241" spans="1:6" ht="15.75" customHeight="1">
+    <row r="241" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="18"/>
       <c r="F241" s="63"/>
     </row>
-    <row r="242" spans="1:6" ht="15.75" customHeight="1">
+    <row r="242" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="18"/>
       <c r="F242" s="63"/>
     </row>
-    <row r="243" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="244" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="245" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="246" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="247" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="248" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="249" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="250" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="251" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="252" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="253" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="254" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="255" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="256" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="243" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="34">
     <mergeCell ref="A1:I1"/>

</xml_diff>

<commit_message>
chore: update 62 btech sem4,2 62 bca sem 4
</commit_message>
<xml_diff>
--- a/raw/time_tables/BCA(bca-62)/4/1.xlsx
+++ b/raw/time_tables/BCA(bca-62)/4/1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\EVEN 2026\2 Year\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\EVEN 2026\2 Year\TT_6JAN\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18161A18-EF03-4B22-8F23-5AA857A62644}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5FC829-F0BF-4FFF-BFE3-5C3B972EB1DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,9 +279,6 @@
     <t>PBCA1(23B65CA224  CL306,)SHR,RTK</t>
   </si>
   <si>
-    <t>PBCA3(23B65CA224) CL304 SHV,NET</t>
-  </si>
-  <si>
     <t>LBCA1,BCA2,BCA 3 &amp;BCA 4(23B12CA216)-MEE/CR526</t>
   </si>
   <si>
@@ -333,20 +330,23 @@
     <t>PBCA3(23B65CA225)/ CL13, CL14/ AJP,NET</t>
   </si>
   <si>
-    <t>PBCA4(23B65CA224) CC 421 RTK,NET</t>
-  </si>
-  <si>
-    <t>PBCA2(23B65CA224)CC417 SHR,RTK</t>
-  </si>
-  <si>
     <t>TBCA2(23B61CA223)-TR502/AJP</t>
+  </si>
+  <si>
+    <t>PBCA3(23B65CA224)-CL14/SHV,NET</t>
+  </si>
+  <si>
+    <t>PBCA4(23B65CA224)-CC421/RTK,NET</t>
+  </si>
+  <si>
+    <t>PBCA2(23B65CA224)-CC417/SHR,KM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -575,8 +575,31 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,12 +636,6 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -1125,9 +1142,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1176,101 +1190,104 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1539,8 +1556,8 @@
   <dimension ref="A1:X993"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="106" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1565,7 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
@@ -1558,17 +1575,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
       <c r="L1" s="18"/>
@@ -1586,17 +1603,17 @@
       <c r="X1" s="18"/>
     </row>
     <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
       <c r="L2" s="18"/>
@@ -1640,59 +1657,59 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="122" t="s">
+    <row r="4" spans="1:24" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="69" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="69" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="69" t="s">
+      <c r="C4" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="69" t="s">
+      <c r="G4" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="113" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" s="114"/>
+      <c r="H4" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="95"/>
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
     </row>
-    <row r="5" spans="1:24" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="122"/>
-      <c r="B5" s="69" t="s">
+    <row r="5" spans="1:24" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="92"/>
+      <c r="B5" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="69" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="69" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="69" t="s">
+      <c r="C5" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="97"/>
-      <c r="G5" s="76" t="s">
+      <c r="F5" s="93"/>
+      <c r="G5" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="1:24" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
       <c r="B6" s="29"/>
       <c r="C6" s="30"/>
@@ -1705,47 +1722,47 @@
       <c r="J6" s="27"/>
       <c r="K6" s="27"/>
     </row>
-    <row r="7" spans="1:24" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="118" t="s">
+    <row r="7" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="117" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="76" t="s">
+      <c r="C7" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="97" t="s">
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="76" t="s">
+      <c r="G7" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="69" t="s">
+      <c r="I7" s="68" t="s">
         <v>80</v>
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
     </row>
-    <row r="8" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="118"/>
-      <c r="B8" s="76" t="s">
+    <row r="8" spans="1:24" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="96"/>
+      <c r="B8" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="113" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="114"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="115" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="116"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
       <c r="J8" s="27"/>
       <c r="K8" s="27"/>
     </row>
@@ -1763,44 +1780,44 @@
       <c r="K9" s="27"/>
     </row>
     <row r="10" spans="1:24" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="119" t="s">
+      <c r="A10" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="116" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="117"/>
-      <c r="D10" s="69" t="s">
+      <c r="B10" s="115" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="116"/>
+      <c r="D10" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="97" t="s">
+      <c r="F10" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="76" t="s">
+      <c r="G10" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="73"/>
-      <c r="I10" s="69" t="s">
+      <c r="H10" s="72"/>
+      <c r="I10" s="68" t="s">
         <v>21</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:24" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="119"/>
-      <c r="B11" s="116" t="s">
+      <c r="A11" s="97"/>
+      <c r="B11" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="117"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="97"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="112"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="99"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
     </row>
@@ -1818,52 +1835,52 @@
       <c r="K12" s="27"/>
     </row>
     <row r="13" spans="1:24" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="96" t="s">
+      <c r="A13" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="76" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="74" t="s">
+      <c r="D13" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="97" t="s">
+      <c r="E13" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="69" t="s">
+      <c r="G13" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="H13" s="75" t="s">
+      <c r="H13" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="I13" s="92" t="s">
-        <v>99</v>
+      <c r="I13" s="68" t="s">
+        <v>98</v>
       </c>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
     </row>
     <row r="14" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="96"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="76" t="s">
+      <c r="A14" s="103"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="69" t="s">
+      <c r="D14" s="70"/>
+      <c r="E14" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="97"/>
-      <c r="G14" s="69" t="s">
+      <c r="F14" s="93"/>
+      <c r="G14" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="104"/>
       <c r="J14" s="27"/>
       <c r="K14" s="27"/>
     </row>
@@ -1881,63 +1898,60 @@
       <c r="K15" s="27"/>
     </row>
     <row r="16" spans="1:24" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="108" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="76" t="s">
+      <c r="B16" s="119" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="120"/>
+      <c r="D16" s="75" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="76" t="s">
-        <v>96</v>
-      </c>
-      <c r="F16" s="77" t="s">
+      <c r="F16" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="91" t="s">
-        <v>104</v>
-      </c>
-      <c r="H16" s="70"/>
-      <c r="I16" s="76"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="75"/>
       <c r="J16" s="27"/>
       <c r="K16" s="27"/>
     </row>
     <row r="17" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="100"/>
-      <c r="B17" s="110" t="s">
+      <c r="A17" s="106"/>
+      <c r="B17" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="112"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="110"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="102" t="s">
-        <v>101</v>
-      </c>
-      <c r="H17" s="103"/>
-      <c r="I17" s="69" t="s">
+      <c r="H17" s="122"/>
+      <c r="I17" s="68" t="s">
         <v>69</v>
       </c>
       <c r="J17" s="27"/>
       <c r="K17" s="27"/>
     </row>
     <row r="18" spans="1:11" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="106"/>
-      <c r="E18" s="107"/>
-      <c r="F18" s="77" t="s">
+      <c r="A18" s="107"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="104" t="s">
+      <c r="G18" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="H18" s="105"/>
-      <c r="I18" s="80"/>
+      <c r="H18" s="122"/>
+      <c r="I18" s="79"/>
       <c r="K18" s="27"/>
     </row>
     <row r="19" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1954,17 +1968,19 @@
       <c r="K19" s="27"/>
     </row>
     <row r="20" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="99" t="s">
+      <c r="A20" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="69" t="s">
+      <c r="B20" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="69" t="s">
+      <c r="C20" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="68"/>
-      <c r="E20" s="71"/>
+      <c r="D20" s="113" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="70"/>
       <c r="F20" s="34"/>
       <c r="G20" s="32"/>
       <c r="H20" s="5"/>
@@ -1973,15 +1989,15 @@
       <c r="K20" s="27"/>
     </row>
     <row r="21" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
-      <c r="B21" s="69" t="s">
+      <c r="A21" s="107"/>
+      <c r="B21" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="69" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
+      <c r="C21" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
       <c r="F21" s="34"/>
       <c r="G21" s="32"/>
       <c r="H21" s="5"/>
@@ -2020,19 +2036,19 @@
       <c r="G23" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="115" t="s">
+      <c r="H23" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="115"/>
+      <c r="I23" s="100"/>
       <c r="J23" s="27"/>
       <c r="K23" s="27"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="42"/>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="83" t="s">
+      <c r="C24" s="82" t="s">
         <v>50</v>
       </c>
       <c r="D24" s="25"/>
@@ -2041,19 +2057,19 @@
       <c r="G24" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="93" t="s">
+      <c r="H24" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="93"/>
+      <c r="I24" s="101"/>
       <c r="J24" s="27"/>
       <c r="K24" s="27"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="42"/>
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="83" t="s">
+      <c r="C25" s="82" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="25"/>
@@ -2062,183 +2078,183 @@
       <c r="G25" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="93" t="s">
+      <c r="H25" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="93"/>
+      <c r="I25" s="101"/>
       <c r="J25" s="27"/>
       <c r="K25" s="27"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="42"/>
-      <c r="B26" s="84" t="s">
+      <c r="B26" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="83" t="s">
+      <c r="C26" s="82" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26" s="43"/>
       <c r="F26" s="44"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="95" t="s">
+      <c r="G26" s="84"/>
+      <c r="H26" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="95"/>
+      <c r="I26" s="102"/>
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="42"/>
-      <c r="B27" s="84" t="s">
+      <c r="B27" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="83" t="s">
+      <c r="C27" s="82" t="s">
         <v>56</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="43"/>
       <c r="F27" s="44"/>
-      <c r="G27" s="86" t="s">
+      <c r="G27" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="87" t="s">
+      <c r="H27" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="87"/>
+      <c r="I27" s="86"/>
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="42"/>
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="82" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="45"/>
       <c r="F28" s="46"/>
-      <c r="G28" s="86" t="s">
+      <c r="G28" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="H28" s="87" t="s">
+      <c r="H28" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="I28" s="87"/>
+      <c r="I28" s="86"/>
       <c r="J28" s="27"/>
       <c r="K28" s="27"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="42"/>
-      <c r="B29" s="84" t="s">
+      <c r="B29" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="82" t="s">
         <v>81</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="45"/>
       <c r="F29" s="46"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="95" t="s">
+      <c r="G29" s="84"/>
+      <c r="H29" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="I29" s="95"/>
+      <c r="I29" s="102"/>
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="42"/>
-      <c r="B30" s="84" t="s">
+      <c r="B30" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="83" t="s">
+      <c r="C30" s="82" t="s">
         <v>60</v>
       </c>
       <c r="D30" s="66"/>
       <c r="E30" s="45"/>
       <c r="F30" s="46"/>
-      <c r="G30" s="86" t="s">
+      <c r="G30" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="86" t="s">
+      <c r="H30" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="88"/>
+      <c r="I30" s="87"/>
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="42"/>
-      <c r="B31" s="84" t="s">
+      <c r="B31" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="83" t="s">
+      <c r="C31" s="82" t="s">
         <v>61</v>
       </c>
       <c r="D31" s="66"/>
       <c r="E31" s="45"/>
       <c r="F31" s="46"/>
-      <c r="G31" s="86" t="s">
+      <c r="G31" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="H31" s="86" t="s">
+      <c r="H31" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="I31" s="89"/>
+      <c r="I31" s="88"/>
       <c r="J31" s="27"/>
       <c r="K31" s="27"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="42"/>
-      <c r="B32" s="84" t="s">
+      <c r="B32" s="111" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="83" t="s">
+      <c r="C32" s="82" t="s">
         <v>63</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="45"/>
       <c r="F32" s="46"/>
-      <c r="G32" s="90" t="s">
+      <c r="G32" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="93" t="s">
+      <c r="H32" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="I32" s="93"/>
+      <c r="I32" s="101"/>
       <c r="J32" s="27"/>
       <c r="K32" s="27"/>
     </row>
     <row r="33" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="47"/>
-      <c r="B33" s="84" t="s">
+      <c r="B33" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="84" t="s">
+      <c r="C33" s="83" t="s">
         <v>64</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="45"/>
       <c r="F33" s="46"/>
-      <c r="G33" s="90" t="s">
+      <c r="G33" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="H33" s="93" t="s">
+      <c r="H33" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="93"/>
+      <c r="I33" s="101"/>
       <c r="J33" s="27"/>
       <c r="K33" s="27"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="48"/>
-      <c r="B34" s="84" t="s">
+      <c r="B34" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="84" t="s">
+      <c r="C34" s="83" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="25"/>
@@ -2247,20 +2263,20 @@
       <c r="G34" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="H34" s="93" t="s">
+      <c r="H34" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="I34" s="93"/>
+      <c r="I34" s="101"/>
       <c r="J34" s="27"/>
       <c r="K34" s="27"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="48"/>
-      <c r="B35" s="84" t="s">
+      <c r="B35" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="83" t="s">
         <v>86</v>
-      </c>
-      <c r="C35" s="84" t="s">
-        <v>87</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="45"/>
@@ -2268,20 +2284,20 @@
       <c r="G35" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="H35" s="93" t="s">
+      <c r="H35" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="I35" s="93"/>
+      <c r="I35" s="101"/>
       <c r="J35" s="27"/>
       <c r="K35" s="27"/>
     </row>
     <row r="36" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="48"/>
-      <c r="B36" s="84" t="s">
+      <c r="B36" s="83" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="83" t="s">
         <v>88</v>
-      </c>
-      <c r="C36" s="84" t="s">
-        <v>89</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="45"/>
@@ -2310,13 +2326,13 @@
       <c r="H38" s="56"/>
       <c r="I38" s="56"/>
       <c r="J38" s="6"/>
-      <c r="Q38" s="81" t="s">
+      <c r="Q38" s="80" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="94"/>
-      <c r="B39" s="94"/>
+      <c r="A39" s="110"/>
+      <c r="B39" s="110"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2331,7 +2347,7 @@
       <c r="N39" s="13"/>
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
-      <c r="Q39" s="82" t="s">
+      <c r="Q39" s="81" t="s">
         <v>39</v>
       </c>
       <c r="R39" s="13"/>
@@ -4098,22 +4114,12 @@
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H32:I32"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="F13:F14"/>
@@ -4126,15 +4132,25 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
     <brk id="37" max="16383" man="1"/>
     <brk id="40" max="16383" man="1"/>

</xml_diff>